<commit_message>
Complete Lab 8 report
</commit_message>
<xml_diff>
--- a/Lab Reports/LabReport8/Lab8_Data.xlsx
+++ b/Lab Reports/LabReport8/Lab8_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abereni4u/Dropbox/Github/PHY121/Lab Reports/LabReport8/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15251DFD-C2D0-6449-BC63-C2E4DED14BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B65552-6DD4-0D41-9C46-F2FD725EEEDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15420" windowHeight="14600" activeTab="1" xr2:uid="{A706FECB-9917-594B-8B19-D8E4EC1BC536}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="15420" windowHeight="14600" activeTab="1" xr2:uid="{A706FECB-9917-594B-8B19-D8E4EC1BC536}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1178,7 +1178,7 @@
                   <c:v>2.5049999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.31619999999999998</c:v>
+                  <c:v>3.335</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4566,14 +4566,14 @@
       <selection activeCell="A15" sqref="A15:F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>0.05</v>
       </c>
@@ -4623,7 +4623,7 @@
         <v>1.0720017463581626</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>0.06</v>
       </c>
@@ -4650,7 +4650,7 @@
         <v>1.0830329302113002</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -4677,7 +4677,7 @@
         <v>1.0704396310882387</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>0.08</v>
       </c>
@@ -4704,12 +4704,12 @@
         <v>1.0626800362878279</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>0.05</v>
       </c>
@@ -4746,7 +4746,7 @@
         <v>32.391656756638248</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>0.06</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>26.316909686652352</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -4786,7 +4786,7 @@
         <v>19.946381355271882</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>0.08</v>
       </c>
@@ -4806,12 +4806,12 @@
         <v>14.107198033189755</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -4832,7 +4832,7 @@
       </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>0.1</v>
       </c>
@@ -4855,7 +4855,7 @@
         <v>0.91382241928635044</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>0.15</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>0.28198738173799437</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>0.2</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>0.50073568788311118</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>0.3</v>
       </c>
@@ -4935,18 +4935,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24404FDE-4B41-6B41-B637-CCBB987C0B5E}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="49" workbookViewId="0">
-      <selection activeCell="O46" sqref="O46"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="50" workbookViewId="0">
+      <selection activeCell="Q38" sqref="Q38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -4970,7 +4970,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>0.05</v>
       </c>
@@ -4993,7 +4993,7 @@
         <v>1.0720000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>0.06</v>
       </c>
@@ -5019,7 +5019,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -5042,7 +5042,7 @@
         <v>1.07</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>0.08</v>
       </c>
@@ -5065,12 +5065,12 @@
         <v>1.0620000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -5087,7 +5087,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>0.05</v>
       </c>
@@ -5104,7 +5104,7 @@
         <v>32.39</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>0.06</v>
       </c>
@@ -5124,7 +5124,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>19.940000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>0.08</v>
       </c>
@@ -5158,12 +5158,12 @@
         <v>14.1</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
@@ -5186,7 +5186,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>0.1</v>
       </c>
@@ -5209,7 +5209,7 @@
         <v>2.145</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>0.15</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>2.629</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>0.2</v>
       </c>
@@ -5258,7 +5258,7 @@
         <v>3.0350000000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>0.3</v>
       </c>
@@ -5272,7 +5272,7 @@
         <v>5.9610000000000003</v>
       </c>
       <c r="E20" s="2">
-        <v>0.31619999999999998</v>
+        <v>3.335</v>
       </c>
       <c r="F20" s="2">
         <v>5.3E-3</v>

</xml_diff>